<commit_message>
updated TestPlan, final submission ZIP
</commit_message>
<xml_diff>
--- a/Assignments/Group_7_TestPlan.xlsx
+++ b/Assignments/Group_7_TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Dokumente\TUT\Embedded Systems and Electronics Productization\Project\MySynth_ELT-23056\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive - TUNI.fi\Embedded Systems and Electronics Productization\Project\MySynth_ELT-23056\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{09673CDE-9B26-4494-B4AB-402C31CFF383}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{811F696A-5FC4-4EF3-8828-C51797B9FACF}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{09673CDE-9B26-4494-B4AB-402C31CFF383}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{62956ED8-593B-4B16-8F79-878EFEB0D071}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{1F5BFFA0-4282-47FF-87C3-4E852344A670}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
   <si>
     <t>Test Id</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Give module &amp; instruction manual to Lecturer. Let him install and use it</t>
+  </si>
+  <si>
+    <t>Done on 15.04.19</t>
+  </si>
+  <si>
+    <t>As expected</t>
   </si>
 </sst>
 </file>
@@ -255,12 +261,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -306,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -322,6 +334,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,7 +712,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A1:H24"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +783,15 @@
       <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -785,6 +809,15 @@
       <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -802,6 +835,15 @@
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -819,6 +861,15 @@
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -836,6 +887,15 @@
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -853,6 +913,15 @@
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -870,6 +939,15 @@
       <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="F9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -887,6 +965,15 @@
       <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -903,6 +990,15 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,6 +1017,15 @@
       <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -938,6 +1043,15 @@
       <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -955,6 +1069,15 @@
       <c r="E14" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -972,6 +1095,15 @@
       <c r="E15" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -989,8 +1121,17 @@
       <c r="E16" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1006,8 +1147,17 @@
       <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1023,8 +1173,17 @@
       <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1040,8 +1199,17 @@
       <c r="E19" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1057,8 +1225,17 @@
       <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1074,8 +1251,17 @@
       <c r="E21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1091,8 +1277,17 @@
       <c r="E22" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1108,8 +1303,17 @@
       <c r="E23" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1125,13 +1329,22 @@
       <c r="E24" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1153,7 +1366,7 @@
           <x14:formula1>
             <xm:f>'.'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>H5:H32</xm:sqref>
+          <xm:sqref>H25:H32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91FCB3EE-117E-494F-95CB-408871798952}">
           <x14:formula1>

</xml_diff>